<commit_message>
credenciales empleado en proceso de foto
</commit_message>
<xml_diff>
--- a/tablaEmpleados_SUIDEV.xlsx
+++ b/tablaEmpleados_SUIDEV.xlsx
@@ -737,8 +737,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1025,16 +1028,24 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="993" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
+    <col min="9" max="10" width="30.42578125" style="1" customWidth="1"/>
+    <col min="11" max="993" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>216369</v>
       </c>
@@ -1059,14 +1070,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>216373</v>
       </c>
@@ -1091,14 +1102,14 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>32716</v>
       </c>
@@ -1123,14 +1134,14 @@
       <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>223003</v>
       </c>
@@ -1155,14 +1166,14 @@
       <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>217331</v>
       </c>
@@ -1187,14 +1198,14 @@
       <c r="H5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>220788</v>
       </c>
@@ -1219,14 +1230,14 @@
       <c r="H6" t="s">
         <v>7</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>215715</v>
       </c>
@@ -1251,14 +1262,14 @@
       <c r="H7" t="s">
         <v>48</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>215270</v>
       </c>
@@ -1283,10 +1294,10 @@
       <c r="H8" t="s">
         <v>54</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1315,14 +1326,14 @@
       <c r="H9" t="s">
         <v>60</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>17053</v>
       </c>
@@ -1347,14 +1358,14 @@
       <c r="H10" t="s">
         <v>65</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>217465</v>
       </c>
@@ -1379,14 +1390,14 @@
       <c r="H11" t="s">
         <v>7</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>217842</v>
       </c>
@@ -1408,14 +1419,14 @@
       <c r="H12" t="s">
         <v>75</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>217984</v>
       </c>
@@ -1440,14 +1451,14 @@
       <c r="H13" t="s">
         <v>60</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>219377</v>
       </c>
@@ -1469,14 +1480,14 @@
       <c r="H14" t="s">
         <v>90</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>223172</v>
       </c>
@@ -1501,14 +1512,14 @@
       <c r="H15" t="s">
         <v>96</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4578</v>
       </c>
@@ -1530,14 +1541,14 @@
       <c r="H16" t="s">
         <v>102</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>215467</v>
       </c>
@@ -1559,14 +1570,14 @@
       <c r="H17" t="s">
         <v>7</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>217848</v>
       </c>
@@ -1591,14 +1602,14 @@
       <c r="H18" t="s">
         <v>112</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>218025</v>
       </c>
@@ -1623,14 +1634,14 @@
       <c r="H19" t="s">
         <v>118</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>219805</v>
       </c>
@@ -1655,14 +1666,14 @@
       <c r="H20" t="s">
         <v>7</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>225277</v>
       </c>
@@ -1687,10 +1698,10 @@
       <c r="H21" t="s">
         <v>7</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1719,10 +1730,10 @@
       <c r="H22" t="s">
         <v>7</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1751,14 +1762,14 @@
       <c r="H23" t="s">
         <v>7</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>222652</v>
       </c>
@@ -1783,14 +1794,14 @@
       <c r="H24" t="s">
         <v>145</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>222704</v>
       </c>
@@ -1815,14 +1826,14 @@
       <c r="H25" t="s">
         <v>151</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>223659</v>
       </c>
@@ -1847,14 +1858,14 @@
       <c r="H26" t="s">
         <v>156</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>222079</v>
       </c>
@@ -1879,14 +1890,14 @@
       <c r="H27" t="s">
         <v>161</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>227702</v>
       </c>
@@ -1911,14 +1922,14 @@
       <c r="H28" t="s">
         <v>7</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>230422</v>
       </c>
@@ -1943,10 +1954,10 @@
       <c r="H29" t="s">
         <v>54</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1975,14 +1986,14 @@
       <c r="H30" t="s">
         <v>112</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>232485</v>
       </c>
@@ -2007,14 +2018,14 @@
       <c r="H31" t="s">
         <v>7</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>232500</v>
       </c>
@@ -2039,14 +2050,14 @@
       <c r="H32" t="s">
         <v>7</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>232492</v>
       </c>
@@ -2071,14 +2082,14 @@
       <c r="H33" t="s">
         <v>102</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>230903</v>
       </c>
@@ -2103,14 +2114,14 @@
       <c r="H34" t="s">
         <v>192</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>232498</v>
       </c>
@@ -2135,14 +2146,14 @@
       <c r="H35" t="s">
         <v>102</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>232490</v>
       </c>
@@ -2167,14 +2178,14 @@
       <c r="H36" t="s">
         <v>102</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>232495</v>
       </c>
@@ -2199,14 +2210,14 @@
       <c r="H37" t="s">
         <v>102</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>232488</v>
       </c>
@@ -2231,10 +2242,10 @@
       <c r="H38" t="s">
         <v>102</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2263,14 +2274,14 @@
       <c r="H39" t="s">
         <v>213</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>234139</v>
       </c>
@@ -2295,14 +2306,14 @@
       <c r="H40" t="s">
         <v>217</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>234950</v>
       </c>
@@ -2327,14 +2338,14 @@
       <c r="H41" t="s">
         <v>7</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>235636</v>
       </c>
@@ -2359,10 +2370,10 @@
       <c r="H42" t="s">
         <v>227</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="1" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>